<commit_message>
Private - public - get - set - pacotes - import
</commit_message>
<xml_diff>
--- a/Funcoes.xlsx
+++ b/Funcoes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3cc209085219c089/Área de Trabalho/Java/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allep\Downloads\Curso-Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="11_AD4D361C20488DEA4E38A0246C9B413A5ADEDD8D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EFE1633-D5CF-4BD4-BC81-B4CA84E8E978}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E880B6-238C-4EE6-AD63-9AB08892BADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
   <si>
     <t>Funcao</t>
   </si>
@@ -298,6 +298,60 @@
   </si>
   <si>
     <t>Lembrar que o void é um metodo que não retorna nada, ele pode ser uma "funcao" apenas para modificar, incrementar... E assim por diante.</t>
+  </si>
+  <si>
+    <t>PRIVATE</t>
+  </si>
+  <si>
+    <t>So pode ler de dentro da classe ou criando um metodo para poder ser lido de fora, exemplo no projeto Screenmatch</t>
+  </si>
+  <si>
+    <t>metodo acessor</t>
+  </si>
+  <si>
+    <t>é para deixar alguem ou outra classe acessar e não alterar.</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>obter valor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET </t>
+  </si>
+  <si>
+    <t>SETAR VALOR, ADICIONAR VALOR, ATRIBUIR VALOR</t>
+  </si>
+  <si>
+    <t>minhaVariavel = 10 || minhaVariavel set 10</t>
+  </si>
+  <si>
+    <t>Packege = PACOTE</t>
+  </si>
+  <si>
+    <t>Organiza codigo pela funcionalidade de suas classes</t>
+  </si>
+  <si>
+    <t>Lembrar que sempre usamos o nome de tras para frente br.com.alleph.screenmatch</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Após criar um pacote precisamos importar eles, observe na parte de cima </t>
+  </si>
+  <si>
+    <t>Package br.com.alleph.screenmatch aqui esta dizendo que essa classe pertence a esse pacote</t>
+  </si>
+  <si>
+    <t>Já no import quer dizer, que essa classe aqui precisa daquela classe la.</t>
+  </si>
+  <si>
+    <t>Classe em outro pacote</t>
+  </si>
+  <si>
+    <t>Lembrar que para usar os atributos precisamos informar que ele e public quando esta em outro pacote</t>
   </si>
 </sst>
 </file>
@@ -672,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -683,7 +737,8 @@
     <col min="1" max="1" width="43.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="87.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="82.42578125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="110" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
@@ -832,7 +887,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
@@ -843,7 +898,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -854,7 +909,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>42</v>
       </c>
@@ -865,7 +920,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>42</v>
       </c>
@@ -876,7 +931,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="3" customFormat="1" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" s="3" customFormat="1" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>42</v>
       </c>
@@ -887,7 +942,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
@@ -898,7 +953,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="3" customFormat="1" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" s="3" customFormat="1" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>42</v>
       </c>
@@ -909,7 +964,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="3" customFormat="1" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" s="3" customFormat="1" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>42</v>
       </c>
@@ -920,7 +975,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>42</v>
       </c>
@@ -931,12 +986,80 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Private - public - get - set - pacotes - import2
</commit_message>
<xml_diff>
--- a/Funcoes.xlsx
+++ b/Funcoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allep\Downloads\Curso-Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E880B6-238C-4EE6-AD63-9AB08892BADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A22E60A-ADB9-4D90-B272-144989752AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
   <si>
     <t>Funcao</t>
   </si>
@@ -352,6 +352,24 @@
   </si>
   <si>
     <t>Lembrar que para usar os atributos precisamos informar que ele e public quando esta em outro pacote</t>
+  </si>
+  <si>
+    <t>Getters</t>
+  </si>
+  <si>
+    <t>Onde eu vou buscar valor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setters </t>
+  </si>
+  <si>
+    <t>Onde eu vou incluir valor</t>
+  </si>
+  <si>
+    <t>Onde eu vou ler o valor da variavel</t>
+  </si>
+  <si>
+    <t>Onde eu posso modificar a variavel</t>
   </si>
 </sst>
 </file>
@@ -726,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -1054,12 +1072,34 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Iniciando o modulo 04
</commit_message>
<xml_diff>
--- a/Funcoes.xlsx
+++ b/Funcoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3cc209085219c089/Área de Trabalho/Curso-Java/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{0A22E60A-ADB9-4D90-B272-144989752AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C37115B5-11ED-48E7-BC72-8100C171EF26}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{0A22E60A-ADB9-4D90-B272-144989752AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FB670FF-20EF-49F8-B768-130CC03A9B0C}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="138">
   <si>
     <t>Funcao</t>
   </si>
@@ -389,12 +389,193 @@
   <si>
     <t>Lembrar que em uma interface todos metodos são como padrao publicos sem precisar escrever o public</t>
   </si>
+  <si>
+    <t>listaDeFilmes.add(filmeDoAlleph);
+        listaDeFilmes.add(meuFilme);
+        listaDeFilmes.add(outroFilme);</t>
+  </si>
+  <si>
+    <t>ArrayList&lt;Filme&gt; listaDeFilmes = new ArrayList&lt;&gt;();    listaDeFilmes.add(filmeDoAlleph);
+        listaDeFilmes.add(meuFilme);
+        listaDeFilmes.add(outroFilme);</t>
+  </si>
+  <si>
+    <t>Criando meu array com a lista de filmes, observa que estamos adicionando os filmes dentro de uma lista</t>
+  </si>
+  <si>
+    <t>Contar quantos elementos tem dentro da lista</t>
+  </si>
+  <si>
+    <t>ArrayList</t>
+  </si>
+  <si>
+    <t>size()</t>
+  </si>
+  <si>
+    <t>listaDeFilmes.get(1).getNome()</t>
+  </si>
+  <si>
+    <t>Pegando o filme elemento 1 e pegando o nome do filme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        System.out.println("Minha lista de filmes: " + listaDeFilmes.get(1).getNome());</t>
+  </si>
+  <si>
+    <t>System.out.println("\n\n\n\nTamanho da lista: " + listaDeFilmes.size() );</t>
+  </si>
+  <si>
+    <t>ToString</t>
+  </si>
+  <si>
+    <t>[br.com.alura.screenmatch.modelos.Filme@7530d0a, br.com.alura.screenmatch.modelos.Filme@34c45dca, br.com.alura.screenmatch.modelos.Filme@52cc8049]</t>
+  </si>
+  <si>
+    <t>Antes ele dava essa informação, ai reescrevemos o metodo para ele da outra informação como.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @Override
+    public String toString() {
+        return "Filme: " + this.getNome() + " (" + this.getAnoDeLancamento() + ")";
+        //return super.toString(); Isso aqui significa, SUPER toString = devolva por padrao oque ja tem na classe mae
+        // Antes ele pegava nome da classe + @ + um codigo hexadecimal
+        // Agora ele pega essa informação que eu escolhi
+    }</t>
+  </si>
+  <si>
+    <t>System.out.println(listaDeFilmes); //     agora formatado da maneira que escolhemos ele vai aparecer assim [Filme: O Senhor dos Aneis (2002), Filme: O poderoso chefão (1970), Filme: Avatar (2023)]</t>
+  </si>
+  <si>
+    <t>super.toString</t>
+  </si>
+  <si>
+    <t>O comando super ele herda/pega a formula que já esta escrita</t>
+  </si>
+  <si>
+    <t>no caso aqui o super.toString ele vai pegar a formula que já esta escrita na classe MAE ou seja a formula que já esta escrito na Classe toString, mas tirando o super vamos reescrever o metodo</t>
+  </si>
+  <si>
+    <t>Construtor</t>
+  </si>
+  <si>
+    <t>O construtor é uma forma de em vez de voce chamar toda vez a variavel e passar um objeto, voce coloca diretamente nela como se fosse um argumento de uma funçao.</t>
+  </si>
+  <si>
+    <t>var filmeDoAlleph = new Filme("O Senhor dos Aneis", 10);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    public Filme(String nomeDoFilme, int notaDoFilme) {
+        this.setNome(nomeDoFilme);
+        this.avalia(notaDoFilme);
+    }</t>
+  </si>
+  <si>
+    <t>Exemplo do construtor, facilitando o codigo.</t>
+  </si>
+  <si>
+    <t>Lembrar que toda classe tem um construtor, mesmo que não colocamos ela, ele cria um por padrao que não é visto aos olhos, então quando criamos uma outra classe que herda ela, se fizer um novo construtor ou seja, ele vai alterar aquele padrao que não estamos vendo, mas esta ali, você também vai precisar criar o mesmo construtor na classe que voce esta herdando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    public Titulo(String nome, int anoDeLancamento){
+        this.nome = nome;
+        this.anoDeLancamento = anoDeLancamento;
+    }</t>
+  </si>
+  <si>
+    <t>Classe serie                          public Serie(String nome, int anoDeLancamento) {
+        super(nome, anoDeLancamento);
+    }</t>
+  </si>
+  <si>
+    <t>Imagina que criamos um construtor na classe titulo, vamos precisar criar na classe que extende a classe titulo que é a classe Serie, observa que ela usa o SUPER</t>
+  </si>
+  <si>
+    <t>super</t>
+  </si>
+  <si>
+    <t>é quando vamos pegar algo da classe mae, a classe que esta mais a cima.</t>
+  </si>
+  <si>
+    <t>Imprimir ArrayList</t>
+  </si>
+  <si>
+    <t>listaDeFilmes.forEach(System.out::println);</t>
+  </si>
+  <si>
+    <t>Outra forma de imprimir toda a lista.</t>
+  </si>
+  <si>
+    <t>Cast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Filme filme = (Filme) item; // Aqui estou dizendo que item é um filme
+            System.out.println("Classificação: " + filme.getClassificacao());</t>
+  </si>
+  <si>
+    <t>Nesse exemplo o filme é uma outra classe. Filme é classe filha de titulo, então a forma de pegar a classificação de filme seria dizendo que ITEM é um FILME dessa forma.</t>
+  </si>
+  <si>
+    <t>Filme filme = (Filme) item</t>
+  </si>
+  <si>
+    <t>Item é um FILME que esta dentro de FILME</t>
+  </si>
+  <si>
+    <t>instanceof</t>
+  </si>
+  <si>
+    <t>Verifcar qual a instancia para evitar erro, se for filme vamos fazer o CAST item é um FILME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            if (item instanceof Filme filme &amp;&amp; filme.getClassificacao() &gt; 2) {
+                System.out.println("Clasificação: " + filme.getClassificacao());
+            }</t>
+  </si>
+  <si>
+    <t>*Antes dava um erro, porque tinha SERIE junto, e ITEM não é SERIE; Item é Filme, ai dava um erro, agora fizemos um if para verificar se Item é Filme, se for imprime o filme.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De quebra ainda colocamos outra condição </t>
+  </si>
+  <si>
+    <t>Collections.sort</t>
+  </si>
+  <si>
+    <t>Ele ordenena uma lista</t>
+  </si>
+  <si>
+    <t>Collections.sort(buscarPorArtistas);
+        System.out.println("Depois da ordenação a lista ficou em: " + buscarPorArtistas);</t>
+  </si>
+  <si>
+    <t>buscaPorArtista é o nome da lista.</t>
+  </si>
+  <si>
+    <t>Lembrar que dessa forma ele funciona apenas com objetos que sabem se comparar um com os outros</t>
+  </si>
+  <si>
+    <t>public class Titulo implements Comparable &lt;Titulo&gt;{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    @Override
+    public int compareTo(Titulo outroTitulo) {
+        return this.getNome().compareTo(outroTitulo.getNome());
+    }</t>
+  </si>
+  <si>
+    <t>O comparable é um comparador para reorganizar a lista, devemos iniciar ele na classe que queremos, e informar qual tipo de dados vamos comparar, se voce observa em baixo eu estou dizendo para:   Pegar o nome 0, comparar com "OUTRO NOME" que vai ser o getNome 1</t>
+  </si>
+  <si>
+    <t>Lembrar que nesse caso eu precisei fazer o toString</t>
+  </si>
+  <si>
+    <t>Comparador(Interface)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,8 +604,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,6 +627,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -471,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -480,6 +691,21 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -766,19 +992,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="53.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="87.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="82.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="110" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="45" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
@@ -1094,7 +1321,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>72</v>
       </c>
@@ -1102,7 +1329,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>74</v>
       </c>
@@ -1113,7 +1340,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>76</v>
       </c>
@@ -1124,7 +1351,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>80</v>
       </c>
@@ -1132,7 +1359,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="69.75" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="69.75" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>82</v>
       </c>
@@ -1144,6 +1371,194 @@
       </c>
       <c r="D37" s="1" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="4" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="7" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="6" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="8" customFormat="1" ht="232.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="93" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="6" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+      <c r="A44" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="6" customFormat="1" ht="162.75" x14ac:dyDescent="0.35">
+      <c r="A45" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="93" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="116.25" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="93" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="116.25" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ultimo modulo do curso de API - Try e catch
</commit_message>
<xml_diff>
--- a/Funcoes.xlsx
+++ b/Funcoes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3cc209085219c089/Área de Trabalho/Curso-Java/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{0A22E60A-ADB9-4D90-B272-144989752AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FB670FF-20EF-49F8-B768-130CC03A9B0C}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="13_ncr:1_{0A22E60A-ADB9-4D90-B272-144989752AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38678A9D-61DA-4BD1-AB4A-2BB80E37DC5E}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="191">
   <si>
     <t>Funcao</t>
   </si>
@@ -568,14 +568,353 @@
     <t>Lembrar que nesse caso eu precisei fazer o toString</t>
   </si>
   <si>
-    <t>Comparador(Interface)</t>
+    <t>Comparador</t>
+  </si>
+  <si>
+    <t>compareTo(Interface)</t>
+  </si>
+  <si>
+    <t>listaDeFilmes.sort(Comparator.comparing(Titulo::getAnoDeLancamento));</t>
+  </si>
+  <si>
+    <t>Aqui estamos pedindo para exibir a lista por ordem em anoDeLancamento</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Request</t>
+  </si>
+  <si>
+    <t>Primeiro precisamos fazer a requisição ou seja oque vai vir.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        // Aqui é o http request
+        HttpClient client = HttpClient.newHttpClient();
+        HttpRequest request = HttpRequest.newBuilder()
+                .uri(URI.create("https://www.omdbapi.com/?t=The+walking+dead&amp;apikey=6e3143f0"))
+                .build();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTTP-Response </t>
+  </si>
+  <si>
+    <t xml:space="preserve">aqui é onde vai ser a resposta do que chegou </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replace </t>
+  </si>
+  <si>
+    <t>entrada: Alleph Nogueira</t>
+  </si>
+  <si>
+    <t>saida: Alleph+Nogueira</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>var nomeFilmeBuscado = leitura.nextLine().replace(" ", "+");</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">             Observa que aqui estamos mudando o espaço pelo  +</t>
+    </r>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/</t>
+  </si>
+  <si>
+    <t>é um site para busca bibliotecas já prontas.</t>
+  </si>
+  <si>
+    <t>Pegando x letras</t>
+  </si>
+  <si>
+    <t>substring(0,2)</t>
+  </si>
+  <si>
+    <t>Imagina que temos o nome alleph</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">a saida entao sera </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>all</t>
+    </r>
+  </si>
+  <si>
+    <t>Record</t>
+  </si>
+  <si>
+    <t>Criando um Record
+Jacqueline: Para fazer essa alternativa, vamos criar um arquivo chamado TituloOmdb dentro da pasta "screenmatch &gt; modelos". Na realidade, o que precisamos? Só queremos fazer tradução de um campo para o outro. Não queremos ter uma classe "TitulosOmdb", instanciar ou mudar essa classe em algum momento. Por isso, não precisamos criar como classe.
+Podemos criar como uma estrutura que teve preview no Java 14 e foi homologada no Java 17, o Record. Nele, só declaramos o cabeçalho, já que é imutável. Pois, não queremos mexer com os dados, simplesmente traduzir para transferir de um lugar para o outro.</t>
+  </si>
+  <si>
+    <t>Lembrar que temos a classe Titulo, mas queremos um record apenas para pegar os dados, e logo mais vamos retornar eles para a classe titulo só que já tratados.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Observe na classe titulo eu pegando os dados e transferindo para ela.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">              public Titulo(TituloOmdb meuTituloOmdb) {
+        this.nome = meuTituloOmdb.title();
+        this.anoDeLancamento = meuTituloOmdb.year();
+        this.duracaoEmMinutos = Integer.parseInt((String) meuTituloOmdb.runtime());
+        //this.duracaoEmMinutos = Integer.valueOf(meuTituloOmdb.runtime().substring(0,2));
+        this.genero = meuTituloOmdb.genre();
+        this.linguagensDisponiveis = meuTituloOmdb.Language();
+    }</t>
+    </r>
+  </si>
+  <si>
+    <t>Catch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isso serve para que o programa não pare de rodar, se caso não tiver o Try e o Catch o programa para de rodar no momento que gerar uma exceção </t>
+  </si>
+  <si>
+    <t>O Try ele vai tentar fazer algo e caso aconteca algo diferente(uma exceção)</t>
+  </si>
+  <si>
+    <t>Vamos capturar essa exceção e colocar uma mensagem.</t>
+  </si>
+  <si>
+    <t>getMessage</t>
+  </si>
+  <si>
+    <t>Ele serve para pegar a mensagem que esta na exceção</t>
+  </si>
+  <si>
+    <t>finally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">É usado para executar um bloco caso aconteça uma exceção ou não, ou seja ele é sempre executado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ele é muito util quando precisamos executar uma informaçao caso der erro ou não, </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">try {
+  metodoQuePodeLancarExcecao();
+  System.out.println("Executou");
+} catch (Exception e) {
+  System.out.println("Deu erro!");
+} finally {
+  System.out.println("Finalizou!");
+}  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Obeserva esse codigo, se não tivesse o finally teriamos que colocar 2x a palavra FINALIZOU tanto no try quando no catch, com o FINALLY só precisamos colocar uma unica vez.  Isso porque o independente se der errado ou certo, ele vai executar o finally também</t>
+    </r>
+  </si>
+  <si>
+    <t>Catch(Exception e)</t>
+  </si>
+  <si>
+    <t>Quando não sabemos qual erro pode chegar, usamos o Exception que é a classe mae dos Exception</t>
+  </si>
+  <si>
+    <t>Isso é um exception generico usado para quando não sabemos qual exceção nosso programa pode dar.</t>
+  </si>
+  <si>
+    <t>IOException</t>
+  </si>
+  <si>
+    <t>indica algum problema relacionado com leitura/escrita de dados.</t>
+  </si>
+  <si>
+    <t>Hierarquia</t>
+  </si>
+  <si>
+    <t>Vamos imaginar duas exceções, mae e filha.   ExceptionMae - ExceptionFilha</t>
+  </si>
+  <si>
+    <t>Se eu usar a exceção mae automaticamente eu vou estar relacionado a filha, se for o inverso eu vou esta relacionado somente a filha</t>
+  </si>
+  <si>
+    <t>Imagina que se eu for casar com a MAE eu vou poder dar ordem na mae e filha, se eu CASAR com a FILHA eu vou poder somente comandar a filha.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> multi-catch</t>
+  </si>
+  <si>
+    <t>Em vez de fazer varios catch podemos fazer somente 1 usando o | segue o exemplo</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SEM O MULTI-CATCH:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> try {
+    metodoQuePodeLancarExcecao();
+} catch (NumberFormatException e) {
+    System.out.println("tratando erro...");
+} catch (IllegalArgumentException e) {
+    System.out.println("tratando erro...");
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>COM O MULTI-CATCH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                               try {
+    metodoQuePodeLancarExcecao();
+} catch (NullPointerException | IllegalArgumentException e) {
+    System.out.println("tratando erro...");
+}</t>
+    </r>
+  </si>
+  <si>
+    <t>Uma observação importante de lembrar, é que o uso de multi-catch só é permitido para exceções que não estão relacionadas por uma hierarquia de herança. Se duas exceções compartilham uma hierarquia de herança, você deve lidar com elas em blocos catch separados.</t>
+  </si>
+  <si>
+    <t>Criando minha exceçao</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> if (meuTituloOmdb.year().length() &gt; 4){
+          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  throw new</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ErroDeConversaoDeAnoException</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>("Não consegui converter o ano porque tem mais de 4 caracteres");
+        }</t>
+    </r>
+  </si>
+  <si>
+    <t>Se o meuTitulo tiver mais de 4 caracteres, vamos entrar na nossa exeção</t>
+  </si>
+  <si>
+    <t>Observar que precisamos criar uma classe da exceção.</t>
+  </si>
+  <si>
+    <t>package br.com.alura.screenmatch.excecao;
+public class ErroDeConversaoDeAnoException extends RuntimeException {
+    private String mensagem;
+    public ErroDeConversaoDeAnoException(String mensagem) {
+        this.mensagem = mensagem;
+    }
+    public String getMensagem() {
+        return this.mensagem;
+    }
+}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,6 +945,39 @@
     </font>
     <font>
       <sz val="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -679,10 +1051,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -708,8 +1081,15 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -992,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -1527,42 +1907,241 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="93" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:5" s="4" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+      <c r="A50" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="116.25" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:5" s="4" customFormat="1" ht="116.25" x14ac:dyDescent="0.35">
+      <c r="A51" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>136</v>
+      <c r="B52" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="7" customFormat="1" ht="162.75" x14ac:dyDescent="0.35">
+      <c r="A54" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="7" customFormat="1" ht="162.75" x14ac:dyDescent="0.35">
+      <c r="A55" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="325.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="4" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A65" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="10" customFormat="1" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A66" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="4" customFormat="1" ht="255.75" x14ac:dyDescent="0.35">
+      <c r="A68" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="10" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A69" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="4" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A70" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="4" customFormat="1" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A71" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="4" customFormat="1" ht="232.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="4" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A59" r:id="rId1" xr:uid="{58393E89-7761-4558-B867-9FC88DE73125}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>